<commit_message>
1402/04/02 17:1747 Adding the application layer and  infrastructure layer with project of infrastructure.EfCore
</commit_message>
<xml_diff>
--- a/Documentation/Timing work.xlsx
+++ b/Documentation/Timing work.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex_khatar\Desktop\SocialNetwork Document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TAMRIN\SocialNetworkAPI\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF6BD3D-2496-4997-A961-98C35F953683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145820D6-793F-4745-A833-A2A6994D4965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A2FFED6A-0DDC-4843-B5E1-44DBC4FD2FF0}"/>
   </bookViews>
   <sheets>
     <sheet name="گزارش کلی" sheetId="6" r:id="rId1"/>
     <sheet name="Timing" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet4" sheetId="4" state="hidden" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="Social_Network">Sheet4!$A$2:$A$14</definedName>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="41">
   <si>
     <t>توضیحات</t>
   </si>
@@ -144,6 +144,15 @@
   </si>
   <si>
     <t>بهبود برنامه طبق فید بک های مهندس شهروز (بستن قسمت ادیت بعد از سیو، عدم نمایش پیام وقتی شما در صفحه چت ایشان نیستید، آپدیت اتوماتیک زمان گذشته از ارسال پیام)</t>
+  </si>
+  <si>
+    <t>SocialNetworkApi</t>
+  </si>
+  <si>
+    <t>Structure of project</t>
+  </si>
+  <si>
+    <t>Implementing layers</t>
   </si>
 </sst>
 </file>
@@ -823,7 +832,7 @@
   <dimension ref="A1:G171"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F19"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1292,7 +1301,9 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
+      <c r="A20" s="6">
+        <v>19</v>
+      </c>
       <c r="B20" s="21"/>
       <c r="C20" s="21"/>
       <c r="D20" s="7"/>
@@ -1340,15 +1351,19 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="21"/>
+      <c r="A24" s="6">
+        <v>211</v>
+      </c>
+      <c r="B24" s="21">
+        <v>45100.625</v>
+      </c>
       <c r="C24" s="21"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
       <c r="F24" s="13"/>
       <c r="G24" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-45100.625</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -3076,68 +3091,78 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A9E2256-D3FF-4F38-B12C-163E006677BE}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
1402/04/11 04:12 Complete the UserApplication test
</commit_message>
<xml_diff>
--- a/Documentation/Timing work.xlsx
+++ b/Documentation/Timing work.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TAMRIN\SocialNetworkAPI\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaeim\source\repos\alimoh1372\SocialNetworkAPI\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618799F3-04AF-4D43-87D2-5EE614F4885D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{A2FFED6A-0DDC-4843-B5E1-44DBC4FD2FF0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="گزارش کلی" sheetId="6" r:id="rId1"/>
@@ -21,7 +20,7 @@
     <definedName name="Social_Network">Sheet4!$A$2:$A$14</definedName>
     <definedName name="SocialNetworkApi">Sheet4!$B$2:$B$13</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="43">
   <si>
     <t>توضیحات</t>
   </si>
@@ -157,12 +156,15 @@
   </si>
   <si>
     <t>انتقال برنامه قبلی به برنامه فعلی و آماده سازی آن برحسب دات نت جدید</t>
+  </si>
+  <si>
+    <t>شروع تست نویسی</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-960429]yyyy/dd/mm\ hh:mm:ss;@"/>
     <numFmt numFmtId="165" formatCode="[$-960429]yyyy/mm/dd\ hh:mm:ss;@"/>
@@ -716,7 +718,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6979C7BB-49DD-4B2B-B223-E70FB219D1F0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
@@ -832,11 +834,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{072EBC7C-5AF1-46C3-A505-6638B2B4A899}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G171"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1319,7 +1321,9 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
+      <c r="A21" s="6">
+        <v>20</v>
+      </c>
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
       <c r="D21" s="7"/>
@@ -1331,7 +1335,9 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
+      <c r="A22" s="6">
+        <v>21</v>
+      </c>
       <c r="B22" s="21"/>
       <c r="C22" s="21"/>
       <c r="D22" s="7"/>
@@ -1343,7 +1349,9 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
+      <c r="A23" s="6">
+        <v>22</v>
+      </c>
       <c r="B23" s="21"/>
       <c r="C23" s="21"/>
       <c r="D23" s="7"/>
@@ -1356,7 +1364,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
-        <v>211</v>
+        <v>23</v>
       </c>
       <c r="B24" s="21">
         <v>45100.625</v>
@@ -1379,7 +1387,9 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
+      <c r="A25" s="6">
+        <v>24</v>
+      </c>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
       <c r="D25" s="7"/>
@@ -1391,7 +1401,9 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
+      <c r="A26" s="6">
+        <v>25</v>
+      </c>
       <c r="B26" s="21"/>
       <c r="C26" s="21"/>
       <c r="D26" s="7"/>
@@ -1403,19 +1415,27 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="21"/>
+      <c r="A27" s="6">
+        <v>26</v>
+      </c>
+      <c r="B27" s="21">
+        <v>45109.351388888892</v>
+      </c>
       <c r="C27" s="21"/>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
-      <c r="F27" s="13"/>
+      <c r="F27" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="G27" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-45109.351388888892</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
+      <c r="A28" s="6">
+        <v>27</v>
+      </c>
       <c r="B28" s="21"/>
       <c r="C28" s="21"/>
       <c r="D28" s="7"/>
@@ -3080,7 +3100,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E23 E25:E28 E24" xr:uid="{7134636C-A79F-433B-886A-B3AFFA854603}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E28">
       <formula1>INDIRECT(D2)</formula1>
     </dataValidation>
   </dataValidations>
@@ -3089,11 +3109,11 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FEE3E4AE-AE62-447B-84FC-AF0217A83A24}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Sheet4!$A$1:$D$1</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D18 D20:D28 D19</xm:sqref>
+          <xm:sqref>D2:D28</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3102,10 +3122,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A9E2256-D3FF-4F38-B12C-163E006677BE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+    <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>